<commit_message>
Move primary and special attacks to their own files.
</commit_message>
<xml_diff>
--- a/ship_stats.xlsx
+++ b/ship_stats.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dan\Desktop\space_shooter_server\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E76003AB-9554-4B5D-BA7B-F5081566C8A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF2BCDA6-85E6-420B-A9EC-371F4AA245EC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="24915" yWindow="-1560" windowWidth="27705" windowHeight="13950" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,10 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="61">
-  <si>
-    <t>scout</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="63">
   <si>
     <t>damage_base</t>
   </si>
@@ -79,9 +76,6 @@
     <t>shield_recharge_growth</t>
   </si>
   <si>
-    <t>gunship</t>
-  </si>
-  <si>
     <t>Damage</t>
   </si>
   <si>
@@ -215,6 +209,18 @@
   </si>
   <si>
     <t>defender1</t>
+  </si>
+  <si>
+    <t>special_base</t>
+  </si>
+  <si>
+    <t>special_growth</t>
+  </si>
+  <si>
+    <t>scout1</t>
+  </si>
+  <si>
+    <t>gunship1</t>
   </si>
 </sst>
 </file>
@@ -230,15 +236,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -326,11 +338,85 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -343,6 +429,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -625,102 +724,103 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AW49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="U3" sqref="U3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="M1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="U4" sqref="U4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30.140625" bestFit="1" customWidth="1"/>
-    <col min="17" max="21" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="26" width="10.7109375" customWidth="1"/>
     <col min="28" max="28" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="7.140625" bestFit="1" customWidth="1"/>
     <col min="30" max="49" width="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
+      <c r="B1" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="E1" t="s">
-        <v>37</v>
-      </c>
-      <c r="F1" t="s">
-        <v>38</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="H1" s="3" t="s">
+      <c r="G1" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="H1" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="I1" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="J1" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="K1" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="L1" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="M1" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="N1" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="O1" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="P1" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q1" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="R1" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="S1" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="T1" s="23" t="s">
+        <v>51</v>
+      </c>
+      <c r="U1" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="V1" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="W1" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="X1" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="Y1" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="Z1" s="24" t="s">
         <v>45</v>
       </c>
-      <c r="K1" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="L1" t="s">
-        <v>15</v>
-      </c>
-      <c r="M1" t="s">
-        <v>59</v>
-      </c>
-      <c r="N1" t="s">
-        <v>58</v>
-      </c>
-      <c r="O1" t="s">
-        <v>57</v>
-      </c>
-      <c r="P1" t="s">
-        <v>56</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="R1" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="S1" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="T1" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="U1" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="V1" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="W1" t="s">
-        <v>50</v>
-      </c>
-      <c r="X1" t="s">
-        <v>49</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>48</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>47</v>
-      </c>
       <c r="AB1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>1</v>
+      <c r="A2" s="19" t="s">
+        <v>0</v>
       </c>
       <c r="B2">
         <v>4</v>
@@ -794,11 +894,11 @@
       <c r="Y2">
         <v>13</v>
       </c>
-      <c r="Z2">
-        <v>17</v>
+      <c r="Z2" s="7">
+        <v>16</v>
       </c>
       <c r="AB2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="AC2">
         <v>0</v>
@@ -865,8 +965,8 @@
       </c>
     </row>
     <row r="3" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>2</v>
+      <c r="A3" s="20" t="s">
+        <v>1</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -940,11 +1040,11 @@
       <c r="Y3">
         <v>3</v>
       </c>
-      <c r="Z3">
+      <c r="Z3" s="7">
         <v>4</v>
       </c>
       <c r="AB3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="AC3">
         <f t="shared" ref="AC3:AW3" si="0">$B$2 + (AC$2 * $B$3)</f>
@@ -1032,8 +1132,8 @@
       </c>
     </row>
     <row r="4" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>3</v>
+      <c r="A4" s="20" t="s">
+        <v>2</v>
       </c>
       <c r="B4">
         <v>300</v>
@@ -1084,16 +1184,16 @@
         <v>300</v>
       </c>
       <c r="R4" s="6">
-        <v>350</v>
+        <v>310</v>
       </c>
       <c r="S4" s="6">
-        <v>400</v>
+        <v>320</v>
       </c>
       <c r="T4" s="6">
-        <v>450</v>
+        <v>330</v>
       </c>
       <c r="U4" s="7">
-        <v>500</v>
+        <v>340</v>
       </c>
       <c r="V4" s="6">
         <v>325</v>
@@ -1107,11 +1207,11 @@
       <c r="Y4" s="11">
         <v>475</v>
       </c>
-      <c r="Z4" s="11">
+      <c r="Z4" s="14">
         <v>525</v>
       </c>
       <c r="AB4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="AC4">
         <f>$B$4 + (AC$2 * $B$5)</f>
@@ -1199,8 +1299,8 @@
       </c>
     </row>
     <row r="5" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>10</v>
+      <c r="A5" s="20" t="s">
+        <v>9</v>
       </c>
       <c r="B5">
         <v>10</v>
@@ -1274,11 +1374,11 @@
       <c r="Y5" s="11">
         <v>15</v>
       </c>
-      <c r="Z5" s="11">
+      <c r="Z5" s="14">
         <v>15</v>
       </c>
       <c r="AB5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="AC5">
         <f>$B$6 - (AC$2 * $B$7)</f>
@@ -1366,8 +1466,8 @@
       </c>
     </row>
     <row r="6" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>4</v>
+      <c r="A6" s="20" t="s">
+        <v>3</v>
       </c>
       <c r="B6">
         <v>2000</v>
@@ -1441,11 +1541,11 @@
       <c r="Y6" s="11">
         <v>1650</v>
       </c>
-      <c r="Z6" s="11">
+      <c r="Z6" s="14">
         <v>1600</v>
       </c>
       <c r="AB6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="AC6">
         <f>$B$8 + (AC$2 * $B$9)</f>
@@ -1533,8 +1633,8 @@
       </c>
     </row>
     <row r="7" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>5</v>
+      <c r="A7" s="20" t="s">
+        <v>4</v>
       </c>
       <c r="B7">
         <v>25</v>
@@ -1608,11 +1708,11 @@
       <c r="Y7" s="11">
         <v>35</v>
       </c>
-      <c r="Z7" s="11">
+      <c r="Z7" s="14">
         <v>40</v>
       </c>
       <c r="AB7" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="AC7">
         <f>$B$10 + (AC$2 * $B$11)</f>
@@ -1700,86 +1800,86 @@
       </c>
     </row>
     <row r="8" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8">
+      <c r="A8" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="3">
         <v>250</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="3">
         <v>300</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="3">
         <v>350</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="3">
         <v>400</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="3">
         <v>450</v>
       </c>
-      <c r="G8" s="5">
+      <c r="G8" s="2">
         <v>300</v>
       </c>
-      <c r="H8" s="6">
+      <c r="H8" s="3">
         <v>350</v>
       </c>
-      <c r="I8" s="6">
+      <c r="I8" s="3">
         <v>400</v>
       </c>
-      <c r="J8" s="6">
+      <c r="J8" s="3">
         <v>450</v>
       </c>
-      <c r="K8" s="7">
+      <c r="K8" s="4">
         <v>500</v>
       </c>
-      <c r="L8">
+      <c r="L8" s="3">
         <v>200</v>
       </c>
-      <c r="M8">
+      <c r="M8" s="3">
         <v>225</v>
       </c>
-      <c r="N8">
+      <c r="N8" s="3">
         <v>250</v>
       </c>
-      <c r="O8">
+      <c r="O8" s="3">
         <v>275</v>
       </c>
-      <c r="P8">
+      <c r="P8" s="3">
         <v>300</v>
       </c>
-      <c r="Q8" s="5">
+      <c r="Q8" s="2">
         <v>200</v>
       </c>
-      <c r="R8" s="6">
+      <c r="R8" s="3">
         <v>225</v>
       </c>
-      <c r="S8" s="6">
+      <c r="S8" s="3">
         <v>250</v>
       </c>
-      <c r="T8" s="6">
+      <c r="T8" s="3">
         <v>275</v>
       </c>
-      <c r="U8" s="7">
+      <c r="U8" s="4">
         <v>300</v>
       </c>
-      <c r="V8" s="6">
+      <c r="V8" s="3">
         <v>220</v>
       </c>
-      <c r="W8" s="11">
+      <c r="W8" s="12">
         <v>270</v>
       </c>
-      <c r="X8" s="11">
+      <c r="X8" s="12">
         <v>290</v>
       </c>
-      <c r="Y8" s="11">
+      <c r="Y8" s="12">
         <v>310</v>
       </c>
-      <c r="Z8" s="11">
+      <c r="Z8" s="13">
         <v>330</v>
       </c>
       <c r="AB8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="AC8">
         <f>$B$12 + (AC$2 * $B$13)</f>
@@ -1867,22 +1967,22 @@
       </c>
     </row>
     <row r="9" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9">
+      <c r="A9" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="6">
         <v>12</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="6">
         <v>14</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="6">
         <v>18</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="6">
         <v>22</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="6">
         <v>25</v>
       </c>
       <c r="G9" s="5">
@@ -1900,19 +2000,19 @@
       <c r="K9" s="7">
         <v>25</v>
       </c>
-      <c r="L9">
+      <c r="L9" s="6">
         <v>12</v>
       </c>
-      <c r="M9">
+      <c r="M9" s="6">
         <v>13</v>
       </c>
-      <c r="N9">
+      <c r="N9" s="6">
         <v>14</v>
       </c>
-      <c r="O9">
+      <c r="O9" s="6">
         <v>15</v>
       </c>
-      <c r="P9">
+      <c r="P9" s="6">
         <v>18</v>
       </c>
       <c r="Q9" s="5">
@@ -1942,11 +2042,11 @@
       <c r="Y9" s="11">
         <v>15</v>
       </c>
-      <c r="Z9" s="11">
+      <c r="Z9" s="14">
         <v>18</v>
       </c>
       <c r="AB9" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="AC9">
         <f>$B$14 - (AC$2 * $B$15)</f>
@@ -2034,22 +2134,22 @@
       </c>
     </row>
     <row r="10" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10">
+      <c r="A10" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="6">
         <v>250</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="6">
         <v>300</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="6">
         <v>350</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="6">
         <v>400</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="6">
         <v>450</v>
       </c>
       <c r="G10" s="5">
@@ -2067,19 +2167,19 @@
       <c r="K10" s="7">
         <v>500</v>
       </c>
-      <c r="L10">
+      <c r="L10" s="6">
         <v>200</v>
       </c>
-      <c r="M10">
+      <c r="M10" s="6">
         <v>225</v>
       </c>
-      <c r="N10">
+      <c r="N10" s="6">
         <v>250</v>
       </c>
-      <c r="O10">
+      <c r="O10" s="6">
         <v>275</v>
       </c>
-      <c r="P10">
+      <c r="P10" s="6">
         <v>300</v>
       </c>
       <c r="Q10" s="5">
@@ -2109,96 +2209,96 @@
       <c r="Y10" s="11">
         <v>310</v>
       </c>
-      <c r="Z10" s="11">
+      <c r="Z10" s="14">
         <v>330</v>
       </c>
     </row>
     <row r="11" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11">
+      <c r="A11" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="9">
         <v>12</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="9">
         <v>14</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="9">
         <v>18</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="9">
         <v>22</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="9">
         <v>25</v>
       </c>
-      <c r="G11" s="5">
+      <c r="G11" s="8">
         <v>14</v>
       </c>
-      <c r="H11" s="6">
+      <c r="H11" s="9">
         <v>14</v>
       </c>
-      <c r="I11" s="6">
+      <c r="I11" s="9">
         <v>18</v>
       </c>
-      <c r="J11" s="6">
+      <c r="J11" s="9">
         <v>22</v>
       </c>
-      <c r="K11" s="7">
+      <c r="K11" s="10">
         <v>25</v>
       </c>
-      <c r="L11">
+      <c r="L11" s="9">
         <v>50</v>
       </c>
-      <c r="M11">
+      <c r="M11" s="9">
         <v>12</v>
       </c>
-      <c r="N11">
+      <c r="N11" s="9">
         <v>14</v>
       </c>
-      <c r="O11">
+      <c r="O11" s="9">
         <v>14</v>
       </c>
-      <c r="P11">
+      <c r="P11" s="9">
         <v>18</v>
       </c>
-      <c r="Q11" s="5">
+      <c r="Q11" s="8">
         <v>12</v>
       </c>
-      <c r="R11" s="6">
+      <c r="R11" s="9">
         <v>12</v>
       </c>
-      <c r="S11" s="6">
+      <c r="S11" s="9">
         <v>14</v>
       </c>
-      <c r="T11" s="6">
+      <c r="T11" s="9">
         <v>14</v>
       </c>
-      <c r="U11" s="7">
+      <c r="U11" s="10">
         <v>18</v>
       </c>
-      <c r="V11" s="6">
+      <c r="V11" s="9">
         <v>12</v>
       </c>
-      <c r="W11" s="11">
+      <c r="W11" s="15">
         <v>13</v>
       </c>
-      <c r="X11" s="11">
+      <c r="X11" s="15">
         <v>14</v>
       </c>
-      <c r="Y11" s="11">
+      <c r="Y11" s="15">
         <v>15</v>
       </c>
-      <c r="Z11" s="11">
+      <c r="Z11" s="16">
         <v>18</v>
       </c>
       <c r="AB11" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>11</v>
+      <c r="A12" s="20" t="s">
+        <v>10</v>
       </c>
       <c r="B12">
         <v>3</v>
@@ -2272,11 +2372,11 @@
       <c r="Y12" s="11">
         <v>6</v>
       </c>
-      <c r="Z12" s="11">
+      <c r="Z12" s="14">
         <v>8</v>
       </c>
       <c r="AB12" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="AC12">
         <v>0</v>
@@ -2343,8 +2443,8 @@
       </c>
     </row>
     <row r="13" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>12</v>
+      <c r="A13" s="20" t="s">
+        <v>11</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -2418,11 +2518,11 @@
       <c r="Y13" s="11">
         <v>2</v>
       </c>
-      <c r="Z13" s="11">
+      <c r="Z13" s="14">
         <v>2</v>
       </c>
       <c r="AB13" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="AC13">
         <f>$C$2 + (AC$2 * $C$3)</f>
@@ -2510,8 +2610,8 @@
       </c>
     </row>
     <row r="14" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>13</v>
+      <c r="A14" s="20" t="s">
+        <v>12</v>
       </c>
       <c r="B14">
         <v>28000</v>
@@ -2585,11 +2685,11 @@
       <c r="Y14" s="11">
         <v>26000</v>
       </c>
-      <c r="Z14" s="11">
+      <c r="Z14" s="14">
         <v>25000</v>
       </c>
       <c r="AB14" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="AC14">
         <f>$C$4 + (AC$2 * $C$5)</f>
@@ -2677,8 +2777,8 @@
       </c>
     </row>
     <row r="15" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>14</v>
+      <c r="A15" s="20" t="s">
+        <v>13</v>
       </c>
       <c r="B15">
         <v>500</v>
@@ -2695,19 +2795,19 @@
       <c r="F15">
         <v>500</v>
       </c>
-      <c r="G15" s="8">
+      <c r="G15" s="5">
         <v>500</v>
       </c>
-      <c r="H15" s="9">
+      <c r="H15" s="6">
         <v>500</v>
       </c>
-      <c r="I15" s="9">
+      <c r="I15" s="6">
         <v>500</v>
       </c>
-      <c r="J15" s="9">
+      <c r="J15" s="6">
         <v>500</v>
       </c>
-      <c r="K15" s="10">
+      <c r="K15" s="7">
         <v>500</v>
       </c>
       <c r="L15">
@@ -2725,19 +2825,19 @@
       <c r="P15">
         <v>500</v>
       </c>
-      <c r="Q15" s="8">
+      <c r="Q15" s="5">
         <v>600</v>
       </c>
-      <c r="R15" s="9">
+      <c r="R15" s="6">
         <v>650</v>
       </c>
-      <c r="S15" s="9">
+      <c r="S15" s="6">
         <v>700</v>
       </c>
-      <c r="T15" s="9">
+      <c r="T15" s="6">
         <v>750</v>
       </c>
-      <c r="U15" s="10">
+      <c r="U15" s="7">
         <v>800</v>
       </c>
       <c r="V15" s="6">
@@ -2752,11 +2852,11 @@
       <c r="Y15">
         <v>575</v>
       </c>
-      <c r="Z15">
+      <c r="Z15" s="7">
         <v>600</v>
       </c>
       <c r="AB15" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="AC15">
         <f>$C$6 - (AC$2 * $C$7)</f>
@@ -2844,8 +2944,86 @@
       </c>
     </row>
     <row r="16" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="A16" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="B16" s="3">
+        <v>0.05</v>
+      </c>
+      <c r="C16" s="3">
+        <v>0.05</v>
+      </c>
+      <c r="D16" s="3">
+        <v>0.05</v>
+      </c>
+      <c r="E16" s="3">
+        <v>0.05</v>
+      </c>
+      <c r="F16" s="3">
+        <v>0.05</v>
+      </c>
+      <c r="G16" s="17">
+        <v>0.01</v>
+      </c>
+      <c r="H16" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="I16" s="12">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="J16" s="12">
+        <v>0.02</v>
+      </c>
+      <c r="K16" s="13">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="L16" s="12">
+        <v>0</v>
+      </c>
+      <c r="M16" s="12">
+        <v>0</v>
+      </c>
+      <c r="N16" s="12">
+        <v>0</v>
+      </c>
+      <c r="O16" s="12">
+        <v>0</v>
+      </c>
+      <c r="P16" s="12">
+        <v>0</v>
+      </c>
+      <c r="Q16" s="17">
+        <v>0</v>
+      </c>
+      <c r="R16" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="S16" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="T16" s="12">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="U16" s="13">
+        <v>0.02</v>
+      </c>
+      <c r="V16" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="W16" s="12">
+        <v>0.01</v>
+      </c>
+      <c r="X16" s="12">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="Y16" s="12">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="Z16" s="13">
+        <v>0.02</v>
+      </c>
       <c r="AB16" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="AC16">
         <f>$C$8 + (AC$2 * $C$9)</f>
@@ -2933,8 +3111,86 @@
       </c>
     </row>
     <row r="17" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="A17" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="B17" s="9">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="C17" s="9">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="D17" s="9">
+        <v>0.01</v>
+      </c>
+      <c r="E17" s="9">
+        <v>0.01</v>
+      </c>
+      <c r="F17" s="9">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="G17" s="18">
+        <v>0.01</v>
+      </c>
+      <c r="H17" s="15">
+        <v>0.01</v>
+      </c>
+      <c r="I17" s="15">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="J17" s="15">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="K17" s="16">
+        <v>0.02</v>
+      </c>
+      <c r="L17" s="15">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="M17" s="15">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="N17" s="15">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="O17" s="15">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="P17" s="15">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="Q17" s="18">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="R17" s="15">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="S17" s="15">
+        <v>0.01</v>
+      </c>
+      <c r="T17" s="15">
+        <v>0.01</v>
+      </c>
+      <c r="U17" s="16">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="V17" s="15">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="W17" s="15">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="X17" s="15">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="Y17" s="15">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="Z17" s="16">
+        <v>0.01</v>
+      </c>
       <c r="AB17" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="AC17">
         <f>$C$10 + (AC$2 * $C$11)</f>
@@ -3022,11 +3278,8 @@
       </c>
     </row>
     <row r="18" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
-        <v>23</v>
-      </c>
       <c r="AB18" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="AC18">
         <f>$C$12 + (AC$2 * $C$13)</f>
@@ -3114,11 +3367,11 @@
       </c>
     </row>
     <row r="19" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>16</v>
+      <c r="B19" t="s">
+        <v>21</v>
       </c>
       <c r="AB19" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="AC19">
         <f>$C$14 - (AC$2 * $C$15)</f>
@@ -3207,23 +3460,23 @@
     </row>
     <row r="20" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="21" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="AB21" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="22" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="AB22" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="AC22">
         <v>0</v>
@@ -3291,10 +3544,10 @@
     </row>
     <row r="23" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="AB23" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="AC23">
         <f>$D$2 + (AC$2 * $D$3)</f>
@@ -3383,10 +3636,10 @@
     </row>
     <row r="24" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="AB24" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="AC24">
         <f>$D$4 + (AC$2 * $D$5)</f>
@@ -3475,10 +3728,10 @@
     </row>
     <row r="25" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="AB25" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="AC25">
         <f>$D$6 - (AC$2 * $D$7)</f>
@@ -3566,8 +3819,11 @@
       </c>
     </row>
     <row r="26" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>20</v>
+      </c>
       <c r="AB26" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="AC26">
         <f>$D$8 + (AC$2 * $D$9)</f>
@@ -3655,11 +3911,8 @@
       </c>
     </row>
     <row r="27" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="D27" t="s">
-        <v>33</v>
-      </c>
       <c r="AB27" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="AC27">
         <f>$D$10 + (AC$2 * $D$11)</f>
@@ -3747,17 +4000,11 @@
       </c>
     </row>
     <row r="28" spans="1:49" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>16</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D28">
-        <v>120</v>
+      <c r="D28" t="s">
+        <v>31</v>
       </c>
       <c r="AB28" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="AC28">
         <f>$D$12 + (AC$2 * $D$13)</f>
@@ -3846,16 +4093,16 @@
     </row>
     <row r="29" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>17</v>
-      </c>
-      <c r="B29" t="s">
-        <v>30</v>
+        <v>14</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="D29">
-        <v>900</v>
+        <v>120</v>
       </c>
       <c r="AB29" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="AC29">
         <f>$D$14 - (AC$2 * $D$15)</f>
@@ -3944,41 +4191,41 @@
     </row>
     <row r="30" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B30" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D30">
-        <v>500</v>
+        <v>900</v>
       </c>
     </row>
     <row r="31" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B31" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D31">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="AB31" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="32" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B32" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D32">
         <v>1000</v>
       </c>
       <c r="AB32" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="AC32">
         <v>0</v>
@@ -4046,16 +4293,16 @@
     </row>
     <row r="33" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>21</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>29</v>
+        <v>18</v>
+      </c>
+      <c r="B33" t="s">
+        <v>26</v>
       </c>
       <c r="D33">
-        <v>65</v>
+        <v>1000</v>
       </c>
       <c r="AB33" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="AC33">
         <f>$E$2 + (AC$2 * $E$3)</f>
@@ -4144,16 +4391,16 @@
     </row>
     <row r="34" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>22</v>
-      </c>
-      <c r="B34" t="s">
-        <v>32</v>
+        <v>19</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>27</v>
       </c>
       <c r="D34">
-        <v>5000</v>
+        <v>65</v>
       </c>
       <c r="AB34" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="AC34">
         <f>$E$4 + (AC$2 * $E$5)</f>
@@ -4241,8 +4488,17 @@
       </c>
     </row>
     <row r="35" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>20</v>
+      </c>
+      <c r="B35" t="s">
+        <v>30</v>
+      </c>
+      <c r="D35">
+        <v>5000</v>
+      </c>
       <c r="AB35" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="AC35">
         <f>$E$6 - (AC$2 * $E$7)</f>
@@ -4331,7 +4587,7 @@
     </row>
     <row r="36" spans="1:49" x14ac:dyDescent="0.25">
       <c r="AB36" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="AC36">
         <f>$E$8 + (AC$2 * $E$9)</f>
@@ -4420,7 +4676,7 @@
     </row>
     <row r="37" spans="1:49" x14ac:dyDescent="0.25">
       <c r="AB37" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="AC37">
         <f>$E$10 + (AC$2 * $E$11)</f>
@@ -4509,7 +4765,7 @@
     </row>
     <row r="38" spans="1:49" x14ac:dyDescent="0.25">
       <c r="AB38" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="AC38">
         <f>$E$12 + (AC$2 * $E$13)</f>
@@ -4598,7 +4854,7 @@
     </row>
     <row r="39" spans="1:49" x14ac:dyDescent="0.25">
       <c r="AB39" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="AC39">
         <f>$E$14 - (AC$2 * $E$15)</f>
@@ -4687,12 +4943,12 @@
     </row>
     <row r="41" spans="1:49" x14ac:dyDescent="0.25">
       <c r="AB41" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="42" spans="1:49" x14ac:dyDescent="0.25">
       <c r="AB42" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="AC42">
         <v>0</v>
@@ -4760,7 +5016,7 @@
     </row>
     <row r="43" spans="1:49" x14ac:dyDescent="0.25">
       <c r="AB43" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="AC43">
         <f>$F$2 + (AC$2 * $F$3)</f>
@@ -4849,7 +5105,7 @@
     </row>
     <row r="44" spans="1:49" x14ac:dyDescent="0.25">
       <c r="AB44" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="AC44">
         <f>$F$4 + (AC$2 * $F$5)</f>
@@ -4938,7 +5194,7 @@
     </row>
     <row r="45" spans="1:49" x14ac:dyDescent="0.25">
       <c r="AB45" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="AC45">
         <f>$F$6 - (AC$2 * $F$7)</f>
@@ -5027,7 +5283,7 @@
     </row>
     <row r="46" spans="1:49" x14ac:dyDescent="0.25">
       <c r="AB46" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="AC46">
         <f>$F$8 + (AC$2 * $F$9)</f>
@@ -5116,7 +5372,7 @@
     </row>
     <row r="47" spans="1:49" x14ac:dyDescent="0.25">
       <c r="AB47" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="AC47">
         <f>$F$10 + (AC$2 * $F$11)</f>
@@ -5205,7 +5461,7 @@
     </row>
     <row r="48" spans="1:49" x14ac:dyDescent="0.25">
       <c r="AB48" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="AC48">
         <f>$F$12 + (AC$2 * $F$13)</f>
@@ -5294,7 +5550,7 @@
     </row>
     <row r="49" spans="28:49" x14ac:dyDescent="0.25">
       <c r="AB49" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="AC49">
         <f>$F$14 - (AC$2 * $F$15)</f>

</xml_diff>